<commit_message>
Review [test]solar_wind ArcGIS projects (VEN, GHA, GEO, FRA, USA, CHN)
</commit_message>
<xml_diff>
--- a/data_country_class_wb/CLASS_2025_10_07.xlsx
+++ b/data_country_class_wb/CLASS_2025_10_07.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjh68\dphil_p1\p1_test\wb_country_class\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjh68\dphil_p1\p1_test\data_country_class_wb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A36D6C-D62A-46A0-AB25-2B72EF0C9573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9263288C-15D2-482B-972F-01E61192CC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1140" windowWidth="26985" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32220" yWindow="2130" windowWidth="33510" windowHeight="19470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of economies" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,32 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-No data in 2025 so used 2024 data. </t>
+No data in FY2025 so used FY2024 data. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D213" authorId="0" shapeId="0" xr:uid="{BAC67A70-30F2-400F-9DD7-EF83D41342B9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jihyeon Jeong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Jihyeon Jeong:
+No data in FY2025 so used FY2019 data (the latest data). </t>
         </r>
       </text>
     </comment>
@@ -79,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9441" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9442" uniqueCount="552">
   <si>
     <t>Economy</t>
   </si>
@@ -2321,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F209" sqref="F209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5734,6 +5759,9 @@
       </c>
       <c r="C213" s="9" t="s">
         <v>29</v>
+      </c>
+      <c r="D213" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="E213" s="9" t="s">
         <v>14</v>

</xml_diff>